<commit_message>
Mise à jour 20 ans
</commit_message>
<xml_diff>
--- a/sources/fiche synthèse.xlsx
+++ b/sources/fiche synthèse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loana\Desktop\Ecole\Portfolio\web\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3CB8CA-5132-41DD-A890-3561E5E5ACBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41289797-81EA-4A01-BC10-8E56732CD63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -82,79 +82,107 @@
     <t>Organiser son développement professionnel</t>
   </si>
   <si>
-    <t>▸Recenser et identifier les ressources numériques 
+    <t>▸Collecter, suivre et orienter des demandes 
+▸Traiter des demandes concernant les services réseau et système, applicatifs
+▸Traiter des demandes concernant les applications</t>
+  </si>
+  <si>
+    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
+▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
+▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
+  </si>
+  <si>
+    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
+▸Planifier les activités
+▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
+  </si>
+  <si>
+    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
+▸Déployer un service
+▸Accompagner les utilisateurs dans la mise en place d’un service</t>
+  </si>
+  <si>
+    <t>▸Mettre en place son environnement d’apprentissage personnel
+▸Mettre en œuvre des outils et stratégies de veille informationnelle
+▸Gérer son identité professionnelle
+▸Développer son projet professionnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation en cours de formation
+</t>
+  </si>
+  <si>
+    <t>Réalisations en cours de stage de première année</t>
+  </si>
+  <si>
+    <t>Réalisations en cours de stage de seconde année</t>
+  </si>
+  <si>
+    <t>Création d'un site vitrine d'une entreprise créatrice de site web</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de l'inventaire du parc informatique d'ipssi mlv
+</t>
+  </si>
+  <si>
+    <t>Gestion d'un projet Web e-commerce sur la vente de produits sportifs</t>
+  </si>
+  <si>
+    <t>du 21/09/22 au 05/10/22</t>
+  </si>
+  <si>
+    <t>du 19/10/22 au 20/10/22</t>
+  </si>
+  <si>
+    <t>☑ SLAM</t>
+  </si>
+  <si>
+    <t>NOM et prénom : ALBIACH Loan</t>
+  </si>
+  <si>
+    <t>Centre de formation : école IPSSI (Marne-la-Vallée)</t>
+  </si>
+  <si>
+    <t>Mise en place d'un outil de veille (Feedly et Google Alert)</t>
+  </si>
+  <si>
+    <t>du 19/11/22 au 20/11/22</t>
+  </si>
+  <si>
+    <t>du 02/11/22 au 11/01/22</t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un serveur d'inventaire GLPI</t>
+  </si>
+  <si>
+    <t>du 01/02/23 au 02/02/23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>▸Recenser et identifier les ressources numériques</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
 ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique
 ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service
 ▸Vérifier les conditions de la continuité d’un service informatique
 ▸Gérer des sauvegardes
 ▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
-  </si>
-  <si>
-    <t>▸Collecter, suivre et orienter des demandes 
-▸Traiter des demandes concernant les services réseau et système, applicatifs
-▸Traiter des demandes concernant les applications</t>
-  </si>
-  <si>
-    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
-▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
-▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
-  </si>
-  <si>
-    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
-▸Planifier les activités
-▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
-  </si>
-  <si>
-    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
-▸Déployer un service
-▸Accompagner les utilisateurs dans la mise en place d’un service</t>
-  </si>
-  <si>
-    <t>▸Mettre en place son environnement d’apprentissage personnel
-▸Mettre en œuvre des outils et stratégies de veille informationnelle
-▸Gérer son identité professionnelle
-▸Développer son projet professionnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisation en cours de formation
-</t>
-  </si>
-  <si>
-    <t>Réalisations en cours de stage de première année</t>
-  </si>
-  <si>
-    <t>Réalisations en cours de stage de seconde année</t>
-  </si>
-  <si>
-    <t>Création d'un site vitrine d'une entreprise créatrice de site web</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisation de l'inventaire du parc informatique d'ipssi mlv
-</t>
-  </si>
-  <si>
-    <t>Gestion d'un projet Web e-commerce sur la vente de produits sportifs</t>
-  </si>
-  <si>
-    <t>du 21/09/22 au 05/10/22</t>
-  </si>
-  <si>
-    <t>du 19/10/22 au 20/10/22</t>
-  </si>
-  <si>
-    <t>du 16/11/22 au xx/xx/xx</t>
-  </si>
-  <si>
-    <t>☑ SLAM</t>
-  </si>
-  <si>
-    <t>NOM et prénom : ALBIACH Loan</t>
-  </si>
-  <si>
-    <t>Centre de formation : école IPSSI (Marne-la-Vallée)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -164,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,6 +254,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -500,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -535,9 +569,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -568,6 +599,12 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,6 +646,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -954,7 +994,7 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="118" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -968,27 +1008,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
@@ -996,40 +1036,40 @@
         <v>3</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="24" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1052,25 +1092,25 @@
       </c>
     </row>
     <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="23" t="s">
         <v>18</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -1109,16 +1149,16 @@
       <c r="AQ6"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="A7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1156,21 +1196,23 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16" t="s">
-        <v>24</v>
+      <c r="F8" s="14"/>
+      <c r="G8" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -1209,20 +1251,20 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17"/>
+      <c r="B9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="16"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1260,20 +1302,20 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="17"/>
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="16"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1311,14 +1353,20 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1356,14 +1404,20 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1401,14 +1455,14 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1446,14 +1500,14 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="16"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1491,14 +1545,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="17"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1536,14 +1590,14 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1581,14 +1635,14 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="17"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1626,16 +1680,16 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
+      <c r="A18" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1673,14 +1727,14 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="17"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="16"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1718,14 +1772,14 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="17"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="16"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1763,14 +1817,14 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="17"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1808,14 +1862,14 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="16"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1853,14 +1907,14 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="17"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="16"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -1898,14 +1952,14 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="17"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="16"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -1943,14 +1997,14 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="16"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -1988,14 +2042,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="17"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="16"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2033,16 +2087,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="A27" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2080,14 +2134,14 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="17"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="16"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2125,14 +2179,14 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="17"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="16"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2170,14 +2224,14 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="17"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="16"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2215,14 +2269,14 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="17"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="16"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2260,14 +2314,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="17"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="16"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2305,14 +2359,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="17"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="16"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2350,14 +2404,14 @@
       <c r="AQ33"/>
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="17"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="16"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2395,14 +2449,14 @@
       <c r="AQ34"/>
     </row>
     <row r="35" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="21"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>

</xml_diff>

<commit_message>
Ajout documentations, veille secondaire, fin de la veille principal
</commit_message>
<xml_diff>
--- a/sources/fiche synthèse.xlsx
+++ b/sources/fiche synthèse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loana\Desktop\Ecole\Portfolio\web\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41289797-81EA-4A01-BC10-8E56732CD63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC9811F-B858-4774-8C79-B6025126CC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
-    <t>SESSION 2022</t>
-  </si>
-  <si>
     <t>Option :</t>
   </si>
   <si>
     <t>▢ SISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
@@ -161,28 +155,39 @@
     <t>du 01/02/23 au 02/02/23</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>▸Recenser et identifier les ressources numériques</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t>▸Recenser et identifier les ressources numériques 
 ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique
 ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service
 ▸Vérifier les conditions de la continuité d’un service informatique
 ▸Gérer des sauvegardes
 ▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
-    </r>
+  </si>
+  <si>
+    <t>AP4</t>
+  </si>
+  <si>
+    <t>Test unitaire</t>
+  </si>
+  <si>
+    <t>Création d'un profil Linkedin</t>
+  </si>
+  <si>
+    <t>Mise en place d'un environnement d'apprentissage personnel</t>
+  </si>
+  <si>
+    <t>Réalisation d'un convertisseur de fichier .csv en javascript</t>
+  </si>
+  <si>
+    <t>Réalisation de composant en VueJS</t>
+  </si>
+  <si>
+    <t>Mise en place de feuilles de styles communes entre les différents projets de l'entreprise</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
+  </si>
+  <si>
+    <t>N° candidat : 02244065393</t>
   </si>
 </sst>
 </file>
@@ -269,7 +274,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -529,12 +534,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -599,15 +632,60 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -616,39 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -994,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="118" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1008,109 +1053,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+    </row>
+    <row r="4" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="25" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="B5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="E6" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="22" t="s">
+      <c r="F6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="G6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="H6" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>18</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -1149,16 +1194,16 @@
       <c r="AQ6"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="A7" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1197,23 +1242,19 @@
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="15" t="s">
-        <v>23</v>
+      <c r="E8" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="15"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1252,16 +1293,16 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="16"/>
@@ -1303,17 +1344,21 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
-        <v>23</v>
+      <c r="E10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10"/>
@@ -1354,18 +1399,18 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1405,16 +1450,16 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="25"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="16"/>
@@ -1455,13 +1500,21 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="A13" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="H13" s="16"/>
       <c r="I13"/>
       <c r="J13"/>
@@ -1500,13 +1553,17 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="H14" s="16"/>
       <c r="I14"/>
       <c r="J14"/>
@@ -1545,14 +1602,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1590,14 +1651,18 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="16"/>
+      <c r="H16" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1680,16 +1745,16 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
+      <c r="A18" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1727,13 +1792,19 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="E19" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="H19" s="16"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -2087,16 +2158,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="A27" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2134,12 +2205,18 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
+      <c r="A28" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="E28" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="G28" s="14"/>
       <c r="H28" s="16"/>
       <c r="I28"/>
@@ -2179,12 +2256,18 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
+      <c r="A29" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="E29" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>21</v>
+      </c>
       <c r="G29" s="14"/>
       <c r="H29" s="16"/>
       <c r="I29"/>
@@ -2586,17 +2669,17 @@
     <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Mise à jour fiche de synthèse
</commit_message>
<xml_diff>
--- a/sources/fiche synthèse.xlsx
+++ b/sources/fiche synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loana\Desktop\Ecole\Portfolio\web\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC038858-57FE-4035-AC68-0C48D5EBF37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4204B179-D5A4-47B7-85B4-A3ACD7D6FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,9 +653,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -664,36 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1039,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="72" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="72" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1053,27 +1053,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="29"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1085,36 +1085,36 @@
       </c>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1137,8 +1137,8 @@
       </c>
     </row>
     <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="11" t="s">
         <v>34</v>
       </c>
@@ -1194,16 +1194,16 @@
       <c r="AQ6"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1745,16 +1745,16 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -2160,16 +2160,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2673,17 +2673,17 @@
     <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>